<commit_message>
"New Commit Added On TimeStamp 01/06/2025 21:59
</commit_message>
<xml_diff>
--- a/ExcelFiles/TestData.xlsx
+++ b/ExcelFiles/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\Ahmedabad\ANKUSH_FRAMEWORK\ExcelFiles\"/>
     </mc:Choice>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="208">
   <si>
     <t>Full Name</t>
   </si>
@@ -635,12 +635,28 @@
   </si>
   <si>
     <t>FormId</t>
+  </si>
+  <si>
+    <t>C:\Users\HP\Documents\Ahmedabad\ANKUSH_FRAMEWORK\ScreenShots\Validation\valdn01_10_2025_09_10_21.png</t>
+  </si>
+  <si>
+    <t>C:\Users\HP\Documents\Ahmedabad\ANKUSH_FRAMEWORK\ScreenShots\Validation\valdn01_10_2025_09_10_59.png</t>
+  </si>
+  <si>
+    <t>C:\Users\HP\Documents\Ahmedabad\ANKUSH_FRAMEWORK\ScreenShots\Validation\valdn01_12_2025_09_12_12.png</t>
+  </si>
+  <si>
+    <t>C:\Users\HP\Documents\Ahmedabad\ANKUSH_FRAMEWORK\ScreenShots\Validation\valdn01_12_2025_09_12_45.png</t>
+  </si>
+  <si>
+    <t>C:\Users\HP\Documents\Ahmedabad\ANKUSH_FRAMEWORK\ScreenShots\Validation\valdn01_13_2025_09_13_26.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1013,13 +1029,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.44140625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="20.5546875"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="24.6640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>201</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -1036,7 +1052,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="0">
         <v>101011</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1053,7 +1069,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="0">
         <v>101012</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1070,7 +1086,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="0">
         <v>101013</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1087,7 +1103,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="0">
         <v>101014</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1104,7 +1120,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="0">
         <v>101015</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1121,7 +1137,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" s="0">
         <v>101016</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1138,7 +1154,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="0">
         <v>101017</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1155,7 +1171,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="A9" s="0">
         <v>101018</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1172,7 +1188,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="A10" s="0">
         <v>101019</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1189,7 +1205,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="A11" s="0">
         <v>101020</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1206,7 +1222,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="A12" s="0">
         <v>101021</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1223,7 +1239,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="A13" s="0">
         <v>101022</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1240,7 +1256,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="A14" s="0">
         <v>101023</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1257,7 +1273,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A15">
+      <c r="A15" s="0">
         <v>101024</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1274,7 +1290,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16">
+      <c r="A16" s="0">
         <v>101025</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1291,7 +1307,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17">
+      <c r="A17" s="0">
         <v>101026</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1308,7 +1324,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18">
+      <c r="A18" s="0">
         <v>101027</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1325,7 +1341,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19">
+      <c r="A19" s="0">
         <v>101028</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1342,7 +1358,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20">
+      <c r="A20" s="0">
         <v>101029</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1359,7 +1375,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A21">
+      <c r="A21" s="0">
         <v>101030</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1394,12 +1410,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="109" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.88671875"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="108.98046875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>202</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -1443,7 +1459,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="0">
         <v>101011</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1482,12 +1498,12 @@
       <c r="M2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N2" t="s">
-        <v>196</v>
+      <c r="N2" t="s" s="0">
+        <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="0">
         <v>101012</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1526,12 +1542,12 @@
       <c r="M3" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="N3" t="s">
-        <v>197</v>
+      <c r="N3" t="s" s="0">
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="0">
         <v>101013</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1570,12 +1586,12 @@
       <c r="M4" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="N4" t="s">
-        <v>198</v>
+      <c r="N4" t="s" s="0">
+        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="0">
         <v>101014</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1614,12 +1630,12 @@
       <c r="M5" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="N5" t="s">
-        <v>199</v>
+      <c r="N5" t="s" s="0">
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="0">
         <v>101015</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1658,12 +1674,12 @@
       <c r="M6" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="N6" t="s">
-        <v>200</v>
+      <c r="N6" t="s" s="0">
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" s="0">
         <v>101016</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1702,12 +1718,12 @@
       <c r="M7" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N7" t="s" s="0">
         <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="0">
         <v>101017</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1746,12 +1762,12 @@
       <c r="M8" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N8" t="s" s="0">
         <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="A9" s="0">
         <v>101018</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1790,12 +1806,12 @@
       <c r="M9" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="N9" t="s">
+      <c r="N9" t="s" s="0">
         <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="A10" s="0">
         <v>101019</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1834,12 +1850,12 @@
       <c r="M10" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="N10" t="s">
+      <c r="N10" t="s" s="0">
         <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="A11" s="0">
         <v>101020</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1878,12 +1894,12 @@
       <c r="M11" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="N11" t="s">
+      <c r="N11" t="s" s="0">
         <v>200</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="A12" s="0">
         <v>101021</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1922,12 +1938,12 @@
       <c r="M12" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="N12" t="s">
+      <c r="N12" t="s" s="0">
         <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="A13" s="0">
         <v>101022</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1966,12 +1982,12 @@
       <c r="M13" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="N13" t="s">
+      <c r="N13" t="s" s="0">
         <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="A14" s="0">
         <v>101023</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -2010,12 +2026,12 @@
       <c r="M14" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="N14" t="s">
+      <c r="N14" t="s" s="0">
         <v>200</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A15">
+      <c r="A15" s="0">
         <v>101024</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -2054,12 +2070,12 @@
       <c r="M15" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="N15" t="s">
+      <c r="N15" t="s" s="0">
         <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16">
+      <c r="A16" s="0">
         <v>101025</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -2098,12 +2114,12 @@
       <c r="M16" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="N16" t="s">
+      <c r="N16" t="s" s="0">
         <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17">
+      <c r="A17" s="0">
         <v>101026</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -2142,12 +2158,12 @@
       <c r="M17" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="N17" t="s">
+      <c r="N17" t="s" s="0">
         <v>200</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18">
+      <c r="A18" s="0">
         <v>101027</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -2186,12 +2202,12 @@
       <c r="M18" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="N18" t="s">
+      <c r="N18" t="s" s="0">
         <v>200</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19">
+      <c r="A19" s="0">
         <v>101028</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -2230,12 +2246,12 @@
       <c r="M19" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="N19" t="s">
+      <c r="N19" t="s" s="0">
         <v>200</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A20">
+      <c r="A20" s="0">
         <v>101029</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -2274,12 +2290,12 @@
       <c r="M20" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="N20" t="s">
+      <c r="N20" t="s" s="0">
         <v>200</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A21">
+      <c r="A21" s="0">
         <v>101030</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -2318,7 +2334,7 @@
       <c r="M21" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="N21" t="s">
+      <c r="N21" t="s" s="0">
         <v>200</v>
       </c>
     </row>

</xml_diff>